<commit_message>
more details about dependencies
</commit_message>
<xml_diff>
--- a/docs/components.xlsx
+++ b/docs/components.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40580" yWindow="5660" windowWidth="18940" windowHeight="15720" tabRatio="500"/>
+    <workbookView xWindow="13040" yWindow="5480" windowWidth="18940" windowHeight="15720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>Demultiplex</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Get run information</t>
   </si>
   <si>
-    <t>Number of reads</t>
-  </si>
-  <si>
     <t>Samples, projects, indexes (sample sheet data)</t>
   </si>
   <si>
@@ -145,6 +142,24 @@
   </si>
   <si>
     <t>Global run stats, demultiplexing stats (for undetermined %), sample sheet or equiv. for project name</t>
+  </si>
+  <si>
+    <t>Number of read cycles and read passes</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>sample sheet, run information (num read passes)</t>
+  </si>
+  <si>
+    <t>fastqc data, file names</t>
+  </si>
+  <si>
+    <t>demultiplexing stats</t>
+  </si>
+  <si>
+    <t>global run stats, demultiplexing stats</t>
   </si>
 </sst>
 </file>
@@ -549,7 +564,7 @@
   <dimension ref="A2:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -566,7 +581,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -577,7 +592,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -588,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -599,7 +614,7 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -610,7 +625,7 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -621,7 +636,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -632,7 +647,7 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -643,7 +658,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -654,7 +669,7 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -665,7 +680,7 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -675,6 +690,9 @@
       <c r="B12" t="s">
         <v>19</v>
       </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
@@ -684,7 +702,7 @@
         <v>26</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -697,6 +715,9 @@
       <c r="C15" t="s">
         <v>27</v>
       </c>
+      <c r="G15" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
@@ -708,8 +729,11 @@
       <c r="C16" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="G16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -717,18 +741,24 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>30</v>
+      </c>
+      <c r="G17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>41</v>
+      </c>
+      <c r="G18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -736,10 +766,13 @@
         <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>31</v>
+      </c>
+      <c r="G19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -747,10 +780,13 @@
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>32</v>
+      </c>
+      <c r="G20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -758,10 +794,13 @@
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>33</v>
+      </c>
+      <c r="G21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1"/>
     </row>
   </sheetData>

</xml_diff>